<commit_message>
updated list of itms.
</commit_message>
<xml_diff>
--- a/Codecademy-Build Websites from Scratch calendar.xlsx
+++ b/Codecademy-Build Websites from Scratch calendar.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chip\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chip\OneDrive\WebProjects\chip-l.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="5459ECDC0360E9695DFA71192E445ED4A4701B45" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2796" yWindow="0" windowWidth="28800" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4194" yWindow="0" windowWidth="49866" windowHeight="16248" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="October" sheetId="1" r:id="rId1"/>
@@ -3075,14 +3076,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyFont="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="3" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="3" applyFont="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -3500,10 +3501,10 @@
         <f ca="1">YEAR(TODAY())</f>
         <v>2017</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="15"/>
+      <c r="D1" s="16"/>
       <c r="E1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3512,10 +3513,10 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="16"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="9" t="s">
         <v>1</v>
       </c>
@@ -3874,8 +3875,8 @@
   </sheetPr>
   <dimension ref="B1:H23"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD22"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3889,10 +3890,10 @@
         <f ca="1">YEAR(TODAY())</f>
         <v>2017</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="15"/>
+      <c r="D1" s="16"/>
       <c r="E1" s="8" t="s">
         <v>0</v>
       </c>
@@ -3901,10 +3902,10 @@
       <c r="B2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="16"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="9" t="s">
         <v>1</v>
       </c>
@@ -4465,7 +4466,7 @@
   </sheetPr>
   <dimension ref="B1:H23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -4476,14 +4477,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="1.5">
-      <c r="B1" s="17">
+      <c r="B1" s="15">
         <f ca="1">YEAR(TODAY())</f>
         <v>2017</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="15"/>
+      <c r="D1" s="16"/>
       <c r="E1" s="14" t="s">
         <v>0</v>
       </c>
@@ -4492,10 +4493,10 @@
       <c r="B2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="16"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="9" t="s">
         <v>1</v>
       </c>
@@ -5071,13 +5072,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="1.5">
-      <c r="B1" s="17">
+      <c r="B1" s="15">
         <v>2018</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15"/>
+      <c r="D1" s="16"/>
       <c r="E1" s="14" t="s">
         <v>0</v>
       </c>
@@ -5086,10 +5087,10 @@
       <c r="B2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="16"/>
+      <c r="D2" s="17"/>
       <c r="E2" s="9" t="s">
         <v>1</v>
       </c>

</xml_diff>